<commit_message>
CHSH studies with new kernel
</commit_message>
<xml_diff>
--- a/scripts/rtg_summary.xlsx
+++ b/scripts/rtg_summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="83">
   <si>
     <t>file</t>
   </si>
@@ -52,52 +52,214 @@
     <t>K_2048_same_rho1p16_a2p55_b1p50_smallt.json</t>
   </si>
   <si>
-    <t>K_2048_same_rho1p16_a2p55_b1p50_tfine.json</t>
-  </si>
-  <si>
     <t>K_4096_same_rho1p16_a2p55_b1p50_smallt.json</t>
   </si>
   <si>
-    <t>K_4096_same_rho1p16_a2p55_b1p50_tfine.json</t>
-  </si>
-  <si>
     <t>K_8192_same_rho1p16_a2p55_b1p50_smallt.json</t>
   </si>
   <si>
-    <t>K_8192_same_rho1p16_a2p55_b1p50_tfine.json</t>
-  </si>
-  <si>
-    <t>chsh_2048_k1.json</t>
-  </si>
-  <si>
-    <t>chsh_4096_k1.json</t>
-  </si>
-  <si>
-    <t>chsh_8192_k1.json</t>
-  </si>
-  <si>
-    <t>corr_omega_4096_k1.json</t>
-  </si>
-  <si>
-    <t>corr_omega_8192_k1.json</t>
+    <t>chsh_4096_k1_opposite_q0p9990.json</t>
+  </si>
+  <si>
+    <t>chsh_4096_k1_opposite_q0p9993.json</t>
+  </si>
+  <si>
+    <t>chsh_4096_k1_opposite_q0p9995.json</t>
+  </si>
+  <si>
+    <t>chsh_4096_k1_opposite_q0p9997.json</t>
+  </si>
+  <si>
+    <t>chsh_4096_k1_opposite_q0p9999.json</t>
+  </si>
+  <si>
+    <t>chsh_4096_k1_phase-opp_q0p9990.json</t>
+  </si>
+  <si>
+    <t>chsh_4096_k1_phase-opp_q0p9993.json</t>
+  </si>
+  <si>
+    <t>chsh_4096_k1_phase-opp_q0p9995.json</t>
+  </si>
+  <si>
+    <t>chsh_4096_k1_phase-opp_q0p9997.json</t>
+  </si>
+  <si>
+    <t>chsh_4096_k1_phase-opp_q0p9999.json</t>
+  </si>
+  <si>
+    <t>chsh_4096_k1_phaseopp_q0p9995.json</t>
+  </si>
+  <si>
+    <t>chsh_4096_k1_phencopp_q0p9995.json</t>
+  </si>
+  <si>
+    <t>chsh_4096_k1_q0p995.json</t>
+  </si>
+  <si>
+    <t>chsh_4096_k1_q0p997.json</t>
+  </si>
+  <si>
+    <t>chsh_4096_k1_q0p998.json</t>
+  </si>
+  <si>
+    <t>chsh_4096_k1_q0p999.json</t>
+  </si>
+  <si>
+    <t>chsh_4096_k1_q0p9995.json</t>
+  </si>
+  <si>
+    <t>chsh_4096_k1_same_q0p9990.json</t>
+  </si>
+  <si>
+    <t>chsh_4096_k1_same_q0p9993.json</t>
+  </si>
+  <si>
+    <t>chsh_4096_k1_same_q0p9995.json</t>
+  </si>
+  <si>
+    <t>chsh_4096_k1_same_q0p9997.json</t>
+  </si>
+  <si>
+    <t>chsh_4096_k1_same_q0p9999.json</t>
+  </si>
+  <si>
+    <t>chsh_8192_k1_opposite_q0p9990.json</t>
+  </si>
+  <si>
+    <t>chsh_8192_k1_opposite_q0p9993.json</t>
+  </si>
+  <si>
+    <t>chsh_8192_k1_opposite_q0p9995.json</t>
+  </si>
+  <si>
+    <t>chsh_8192_k1_opposite_q0p9997.json</t>
+  </si>
+  <si>
+    <t>chsh_8192_k1_opposite_q0p9999.json</t>
+  </si>
+  <si>
+    <t>chsh_8192_k1_phase-opp_q0p9990.json</t>
+  </si>
+  <si>
+    <t>chsh_8192_k1_phase-opp_q0p9993.json</t>
+  </si>
+  <si>
+    <t>chsh_8192_k1_phase-opp_q0p9995.json</t>
+  </si>
+  <si>
+    <t>chsh_8192_k1_phase-opp_q0p9997.json</t>
+  </si>
+  <si>
+    <t>chsh_8192_k1_phase-opp_q0p9999.json</t>
+  </si>
+  <si>
+    <t>chsh_8192_k1_phaseopp_q0p9995.json</t>
+  </si>
+  <si>
+    <t>chsh_8192_k1_phencopp_q0p9995.json</t>
+  </si>
+  <si>
+    <t>chsh_8192_k1_same_q0p9990.json</t>
+  </si>
+  <si>
+    <t>chsh_8192_k1_same_q0p9993.json</t>
+  </si>
+  <si>
+    <t>chsh_8192_k1_same_q0p9995.json</t>
+  </si>
+  <si>
+    <t>chsh_8192_k1_same_q0p9997.json</t>
+  </si>
+  <si>
+    <t>chsh_8192_k1_same_q0p9999.json</t>
   </si>
   <si>
     <t>curv_4096_k1_curv_summary.json</t>
   </si>
   <si>
+    <t>curv_4096_k1_opposite_q0p9990_curv_summary.json</t>
+  </si>
+  <si>
+    <t>curv_4096_k1_opposite_q0p9995_curv_summary.json</t>
+  </si>
+  <si>
+    <t>curv_4096_k1_q0p9990_curv_summary.json</t>
+  </si>
+  <si>
+    <t>curv_4096_k1_q0p9995_curv_summary.json</t>
+  </si>
+  <si>
+    <t>curv_4096_k1_same_q0p9990_curv_summary.json</t>
+  </si>
+  <si>
+    <t>curv_4096_k1_same_q0p9995_curv_summary.json</t>
+  </si>
+  <si>
     <t>curv_8192_k1_curv_summary.json</t>
   </si>
   <si>
-    <t>eft_k1.json</t>
-  </si>
-  <si>
-    <t>eft_k1_smallt_window.json</t>
+    <t>curv_8192_k1_opposite_q0p9990_curv_summary.json</t>
+  </si>
+  <si>
+    <t>curv_8192_k1_opposite_q0p9995_curv_summary.json</t>
+  </si>
+  <si>
+    <t>curv_8192_k1_q0p9990_curv_summary.json</t>
+  </si>
+  <si>
+    <t>curv_8192_k1_q0p9995_curv_summary.json</t>
+  </si>
+  <si>
+    <t>curv_8192_k1_same_q0p9990_curv_summary.json</t>
+  </si>
+  <si>
+    <t>curv_8192_k1_same_q0p9995_curv_summary.json</t>
+  </si>
+  <si>
+    <t>eft_4096_k1.json</t>
   </si>
   <si>
     <t>homology_4096_k1_homology_summary.json</t>
   </si>
   <si>
+    <t>homology_4096_k1_opposite_q0p9990_homology_summary.json</t>
+  </si>
+  <si>
+    <t>homology_4096_k1_opposite_q0p9995_homology_summary.json</t>
+  </si>
+  <si>
+    <t>homology_4096_k1_q0p9990_homology_summary.json</t>
+  </si>
+  <si>
+    <t>homology_4096_k1_q0p9995_homology_summary.json</t>
+  </si>
+  <si>
+    <t>homology_4096_k1_same_q0p9990_homology_summary.json</t>
+  </si>
+  <si>
+    <t>homology_4096_k1_same_q0p9995_homology_summary.json</t>
+  </si>
+  <si>
     <t>homology_8192_k1_homology_summary.json</t>
+  </si>
+  <si>
+    <t>homology_8192_k1_opposite_q0p9990_homology_summary.json</t>
+  </si>
+  <si>
+    <t>homology_8192_k1_opposite_q0p9995_homology_summary.json</t>
+  </si>
+  <si>
+    <t>homology_8192_k1_q0p9990_homology_summary.json</t>
+  </si>
+  <si>
+    <t>homology_8192_k1_q0p9995_homology_summary.json</t>
+  </si>
+  <si>
+    <t>homology_8192_k1_same_q0p9990_homology_summary.json</t>
+  </si>
+  <si>
+    <t>homology_8192_k1_same_q0p9995_homology_summary.json</t>
   </si>
   <si>
     <t>same</t>
@@ -458,7 +620,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -516,7 +678,7 @@
         <v>0.55</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="G2">
         <v>-0.01174207563348846</v>
@@ -539,7 +701,7 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>2048</v>
+        <v>4096</v>
       </c>
       <c r="C3">
         <v>1.5</v>
@@ -551,22 +713,22 @@
         <v>0.55</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="G3">
-        <v>-0.05266370485830537</v>
+        <v>-0.04355970028418384</v>
       </c>
       <c r="H3">
-        <v>0.0001406943011551073</v>
+        <v>0.0001456463839842607</v>
       </c>
       <c r="I3">
-        <v>0.9433317132219565</v>
+        <v>0.9662998333841258</v>
       </c>
       <c r="J3">
-        <v>0.01319109769642277</v>
+        <v>0.01106000289363457</v>
       </c>
       <c r="K3">
-        <v>0.05937071610160926</v>
+        <v>0.0580767609974866</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -574,7 +736,7 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <v>4096</v>
+        <v>8192</v>
       </c>
       <c r="C4">
         <v>1.5</v>
@@ -586,128 +748,38 @@
         <v>0.55</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="G4">
-        <v>-0.04355970028418384</v>
+        <v>-0.07477039155646943</v>
       </c>
       <c r="H4">
-        <v>0.0001456463839842607</v>
+        <v>0.0001403975667087544</v>
       </c>
       <c r="I4">
-        <v>0.9662998333841258</v>
+        <v>0.9791606876635998</v>
       </c>
       <c r="J4">
-        <v>0.01106000289363457</v>
+        <v>0.01991609552966864</v>
       </c>
       <c r="K4">
-        <v>0.0580767609974866</v>
+        <v>0.1046568514482464</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5">
-        <v>4096</v>
-      </c>
-      <c r="C5">
-        <v>1.5</v>
-      </c>
-      <c r="D5">
-        <v>1.16</v>
-      </c>
-      <c r="E5">
-        <v>0.55</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5">
-        <v>-0.1489129395916517</v>
-      </c>
-      <c r="H5">
-        <v>0.0008342480801961683</v>
-      </c>
-      <c r="I5">
-        <v>0.9662998333841258</v>
-      </c>
-      <c r="J5">
-        <v>0.03693690502834353</v>
-      </c>
-      <c r="K5">
-        <v>0.1678061667842471</v>
-      </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6">
-        <v>8192</v>
-      </c>
-      <c r="C6">
-        <v>1.5</v>
-      </c>
-      <c r="D6">
-        <v>1.16</v>
-      </c>
-      <c r="E6">
-        <v>0.55</v>
-      </c>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6">
-        <v>-0.07477039155646943</v>
-      </c>
-      <c r="H6">
-        <v>0.0001403975667087544</v>
-      </c>
-      <c r="I6">
-        <v>0.9791606876635998</v>
-      </c>
-      <c r="J6">
-        <v>0.01991609552966864</v>
-      </c>
-      <c r="K6">
-        <v>0.1046568514482464</v>
-      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7">
-        <v>8192</v>
-      </c>
-      <c r="C7">
-        <v>1.5</v>
-      </c>
-      <c r="D7">
-        <v>1.16</v>
-      </c>
-      <c r="E7">
-        <v>0.55</v>
-      </c>
-      <c r="F7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7">
-        <v>-0.242612534585944</v>
-      </c>
-      <c r="H7">
-        <v>0.0007730618374032224</v>
-      </c>
-      <c r="I7">
-        <v>0.9791606876635998</v>
-      </c>
-      <c r="J7">
-        <v>0.06446540831177416</v>
-      </c>
-      <c r="K7">
-        <v>0.2936722444479341</v>
-      </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
@@ -762,6 +834,291 @@
     <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58">
+        <v>4096</v>
+      </c>
+      <c r="C58">
+        <v>1.5</v>
+      </c>
+      <c r="D58">
+        <v>1.16</v>
+      </c>
+      <c r="E58">
+        <v>0.55</v>
+      </c>
+      <c r="F58" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>